<commit_message>
removed spaces from header names
</commit_message>
<xml_diff>
--- a/final_project_covid_data.xlsx
+++ b/final_project_covid_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\School\Spring 2021\Repositories\CovidCasesVsPopulationDensity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32FDA04-C6F3-4DC8-B67A-14737349EA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3762F7B0-8454-4AE0-9F37-DB123E191614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{D22F2606-E809-4BCC-A53E-A1A51CE11D88}"/>
   </bookViews>
@@ -42,18 +42,9 @@
     <t>County</t>
   </si>
   <si>
-    <t>Population density (people/sq km)</t>
-  </si>
-  <si>
     <t>Population</t>
   </si>
   <si>
-    <t>Total COVID cases (as of March 8, 2021)</t>
-  </si>
-  <si>
-    <t>Percentage of population to test positive</t>
-  </si>
-  <si>
     <t>Massachussetts</t>
   </si>
   <si>
@@ -247,6 +238,15 @@
   </si>
   <si>
     <t>Providence</t>
+  </si>
+  <si>
+    <t>Percentage positive</t>
+  </si>
+  <si>
+    <t>PplPerSqMi</t>
+  </si>
+  <si>
+    <t>TotalCovidCases</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,24 +624,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <v>1507.36</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>1210.69</v>
@@ -680,10 +680,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>192.24</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>437.49</v>
@@ -722,10 +722,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>1406.67</v>
@@ -743,10 +743,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>395.49</v>
@@ -764,10 +764,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
       </c>
       <c r="C8">
         <v>367.52</v>
@@ -785,10 +785,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>226.65</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>232.95</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>9.9700000000000006</v>
@@ -848,10 +848,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C12">
         <v>356.19</v>
@@ -869,10 +869,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>18.13</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C14">
         <v>34.97</v>
@@ -911,10 +911,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15">
         <v>141.58000000000001</v>
@@ -932,10 +932,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C16">
         <v>109.23</v>
@@ -953,10 +953,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C17">
         <v>77.010000000000005</v>
@@ -974,10 +974,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C18">
         <v>28.13</v>
@@ -995,10 +995,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C19">
         <v>44.98</v>
@@ -1016,10 +1016,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
         <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
       </c>
       <c r="C20">
         <v>4.26</v>
@@ -1037,10 +1037,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C21">
         <v>142.47999999999999</v>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22">
         <v>12.86</v>
@@ -1079,10 +1079,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23">
         <v>54.57</v>
@@ -1100,10 +1100,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>12.29</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C25">
         <v>213.15</v>
@@ -1142,10 +1142,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C26">
         <v>538.53</v>
@@ -1163,10 +1163,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>132.74</v>
@@ -1184,10 +1184,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C28">
         <v>1025.92</v>
@@ -1205,10 +1205,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C29">
         <v>167.9</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <v>1605.43</v>
@@ -1247,10 +1247,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>99.12</v>
@@ -1268,10 +1268,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C32">
         <v>749.15</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
         <v>6</v>
-      </c>
-      <c r="B33" t="s">
-        <v>9</v>
       </c>
       <c r="C33">
         <v>303.86</v>
@@ -1310,10 +1310,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C34">
         <v>1978.62</v>
@@ -1331,10 +1331,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C35">
         <v>255.92</v>
@@ -1352,10 +1352,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C36">
         <v>1802.18</v>
@@ -1373,10 +1373,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C37">
         <v>799.19</v>
@@ -1394,10 +1394,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C38">
         <v>13825.77</v>
@@ -1415,10 +1415,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C39">
         <v>551.9</v>
@@ -1436,10 +1436,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C40">
         <v>153.96</v>
@@ -1457,10 +1457,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
         <v>41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>44</v>
       </c>
       <c r="C41">
         <v>52.87</v>
@@ -1478,10 +1478,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>108.18</v>
@@ -1499,10 +1499,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C43">
         <v>17.670000000000002</v>
@@ -1520,10 +1520,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C44">
         <v>52.82</v>
@@ -1541,10 +1541,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C45">
         <v>481.41</v>
@@ -1562,10 +1562,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C46">
         <v>163.65</v>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C47">
         <v>450.05</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C48">
         <v>358.66</v>
@@ -1625,10 +1625,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C49">
         <v>80.42</v>
@@ -1646,10 +1646,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C50">
         <v>1994.24</v>
@@ -1667,10 +1667,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C51">
         <v>977.63</v>
@@ -1688,10 +1688,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C52">
         <v>792.48</v>
@@ -1709,10 +1709,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
         <v>67</v>
-      </c>
-      <c r="B53" t="s">
-        <v>70</v>
       </c>
       <c r="C53">
         <v>1569.88</v>
@@ -1730,10 +1730,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C54">
         <v>378.21</v>
@@ -1751,10 +1751,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C55">
         <v>47.74</v>
@@ -1772,10 +1772,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C56">
         <v>52.4</v>
@@ -1793,10 +1793,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C57">
         <v>45.47</v>
@@ -1814,10 +1814,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
         <v>21</v>
-      </c>
-      <c r="B58" t="s">
-        <v>24</v>
       </c>
       <c r="C58">
         <v>305.97000000000003</v>
@@ -1835,10 +1835,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C59">
         <v>9.07</v>
@@ -1856,10 +1856,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C60">
         <v>78.400000000000006</v>
@@ -1877,10 +1877,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C61">
         <v>91.49</v>
@@ -1898,10 +1898,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C62">
         <v>55.56</v>
@@ -1919,10 +1919,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C63">
         <v>42.06</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C64">
         <v>39.49</v>
@@ -1961,10 +1961,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C65">
         <v>61.71</v>
@@ -1982,10 +1982,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C66">
         <v>85.98</v>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C67">
         <v>52.71</v>
@@ -2024,10 +2024,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C68">
         <v>56.51</v>

</xml_diff>

<commit_message>
Finished Q1 a, b, and c
</commit_message>
<xml_diff>
--- a/final_project_covid_data.xlsx
+++ b/final_project_covid_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\School\Spring 2021\Repositories\CovidCasesVsPopulationDensity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3762F7B0-8454-4AE0-9F37-DB123E191614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91096085-F904-4F50-B9D3-6C5E3E586639}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{D22F2606-E809-4BCC-A53E-A1A51CE11D88}"/>
   </bookViews>
@@ -240,13 +240,13 @@
     <t>Providence</t>
   </si>
   <si>
-    <t>Percentage positive</t>
-  </si>
-  <si>
     <t>PplPerSqMi</t>
   </si>
   <si>
     <t>TotalCovidCases</t>
+  </si>
+  <si>
+    <t>PercentagePositive</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,16 +624,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Q2 of project
</commit_message>
<xml_diff>
--- a/final_project_covid_data.xlsx
+++ b/final_project_covid_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\School\Spring 2021\Repositories\CovidCasesVsPopulationDensity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoinj\Documents\Classes\Prob and Stat\Final\CovidCasesVsPopulationDensity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91096085-F904-4F50-B9D3-6C5E3E586639}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666D3199-FA47-4F96-934B-EEF872B6241F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{D22F2606-E809-4BCC-A53E-A1A51CE11D88}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D22F2606-E809-4BCC-A53E-A1A51CE11D88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,13 +240,13 @@
     <t>Providence</t>
   </si>
   <si>
-    <t>PplPerSqMi</t>
-  </si>
-  <si>
     <t>TotalCovidCases</t>
   </si>
   <si>
     <t>PercentagePositive</t>
+  </si>
+  <si>
+    <t>PplPerSqKm</t>
   </si>
 </sst>
 </file>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA85A18-2B65-4D7F-877E-A9AC056809C3}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,16 +624,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1400,7 +1400,7 @@
         <v>11</v>
       </c>
       <c r="C38">
-        <v>13825.77</v>
+        <v>5360</v>
       </c>
       <c r="D38">
         <v>805427</v>

</xml_diff>